<commit_message>
changed additional task1-2, changed basic3
</commit_message>
<xml_diff>
--- a/practice1/basic3.xlsx
+++ b/practice1/basic3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\SQLNeto\practice1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4D0762-7064-42A3-8E12-A6F775E92A25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3017B6B0-5434-4131-8B42-D6B0D493C06E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{94D73617-3141-4094-BE50-85FDED209676}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Название таблицы</t>
   </si>
@@ -91,6 +91,51 @@
   </si>
   <si>
     <t>Как это сделать?</t>
+  </si>
+  <si>
+    <t>actor_id</t>
+  </si>
+  <si>
+    <t>address_id</t>
+  </si>
+  <si>
+    <t>category_id</t>
+  </si>
+  <si>
+    <t>city_id</t>
+  </si>
+  <si>
+    <t>country_id</t>
+  </si>
+  <si>
+    <t>customer_id</t>
+  </si>
+  <si>
+    <t>film_id</t>
+  </si>
+  <si>
+    <t>inventory_id</t>
+  </si>
+  <si>
+    <t>language_id</t>
+  </si>
+  <si>
+    <t>payment_id</t>
+  </si>
+  <si>
+    <t>rental_id</t>
+  </si>
+  <si>
+    <t>staff_id</t>
+  </si>
+  <si>
+    <t>store_id</t>
+  </si>
+  <si>
+    <t>actor_id\film_id</t>
+  </si>
+  <si>
+    <t>film_id\category_id</t>
   </si>
 </sst>
 </file>
@@ -476,7 +521,7 @@
   <dimension ref="A2:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -502,7 +547,9 @@
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="E3" t="s">
         <v>17</v>
       </c>
@@ -514,7 +561,9 @@
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
@@ -523,7 +572,9 @@
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="E5" t="s">
         <v>18</v>
       </c>
@@ -535,7 +586,9 @@
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
@@ -544,7 +597,9 @@
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="1"/>
+      <c r="C7" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
@@ -553,7 +608,9 @@
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="1"/>
+      <c r="C8" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
@@ -562,7 +619,9 @@
       <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
@@ -571,7 +630,9 @@
       <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
@@ -580,7 +641,9 @@
       <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
@@ -589,7 +652,9 @@
       <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
@@ -598,7 +663,9 @@
       <c r="B13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
@@ -607,7 +674,9 @@
       <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="1"/>
+      <c r="C14" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
@@ -616,7 +685,9 @@
       <c r="B15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="1"/>
+      <c r="C15" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
@@ -625,7 +696,9 @@
       <c r="B16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="1"/>
+      <c r="C16" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
@@ -634,7 +707,9 @@
       <c r="B17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="1"/>
+      <c r="C17" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B18" s="2"/>

</xml_diff>